<commit_message>
Fixed repr curves filter combinations.
</commit_message>
<xml_diff>
--- a/examples/baron study/info/03 repr info.xlsx
+++ b/examples/baron study/info/03 repr info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,25 +436,977 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>test id</t>
+          <t>repr id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>material</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>rate</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>temperature</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>repr_id_0000</t>
+          <t>repr_id_0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>AC</t>
         </is>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>repr_id_0002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>repr_id_0003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>repr_id_0004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>repr_id_0007</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>repr_id_0008</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>repr_id_0009</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>repr_id_0010</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>repr_id_0011</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>repr_id_0012</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>repr_id_0016</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>repr_id_0017</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>repr_id_0018</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>repr_id_0019</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50</v>
+      </c>
+      <c r="D15" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>repr_id_0020</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>repr_id_0021</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>50</v>
+      </c>
+      <c r="D17" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>repr_id_0022</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>50</v>
+      </c>
+      <c r="D18" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>repr_id_0025</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>repr_id_0026</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>repr_id_0027</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>repr_id_0028</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>repr_id_0031</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>repr_id_0032</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>10</v>
+      </c>
+      <c r="D24" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>repr_id_0033</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>10</v>
+      </c>
+      <c r="D25" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>repr_id_0034</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>repr_id_0035</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
+      <c r="D27" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>repr_id_0036</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>10</v>
+      </c>
+      <c r="D28" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>repr_id_0039</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>repr_id_0040</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>repr_id_0041</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>repr_id_0042</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>repr_id_0043</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>50</v>
+      </c>
+      <c r="D33" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>repr_id_0044</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>50</v>
+      </c>
+      <c r="D34" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>repr_id_0045</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>50</v>
+      </c>
+      <c r="D35" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>repr_id_0046</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>H560</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>50</v>
+      </c>
+      <c r="D36" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>repr_id_0049</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>100</v>
+      </c>
+      <c r="D37" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>repr_id_0050</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>100</v>
+      </c>
+      <c r="D38" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>repr_id_0051</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>100</v>
+      </c>
+      <c r="D39" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>repr_id_0052</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>100</v>
+      </c>
+      <c r="D40" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>repr_id_0055</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>10</v>
+      </c>
+      <c r="D41" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>repr_id_0056</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>10</v>
+      </c>
+      <c r="D42" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>repr_id_0057</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>10</v>
+      </c>
+      <c r="D43" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>repr_id_0058</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>10</v>
+      </c>
+      <c r="D44" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>repr_id_0059</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>10</v>
+      </c>
+      <c r="D45" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>repr_id_0060</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>10</v>
+      </c>
+      <c r="D46" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>repr_id_0063</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>repr_id_0064</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>repr_id_0065</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>repr_id_0066</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>repr_id_0067</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>50</v>
+      </c>
+      <c r="D51" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>repr_id_0068</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>50</v>
+      </c>
+      <c r="D52" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>repr_id_0069</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>50</v>
+      </c>
+      <c r="D53" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>repr_id_0070</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>H580</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>50</v>
+      </c>
+      <c r="D54" t="n">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>